<commit_message>
Output file path is removed from Input sheet for NI Scenarios
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XCD HR_Documents\Project Imp Documents\Regression Testing_2018_2019\New Input Files_2018_2019\2 Weekly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
-    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
-    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
+    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="62">
   <si>
     <t>TC</t>
   </si>
@@ -126,9 +126,6 @@
     <t>FirstReportNameInApplication</t>
   </si>
   <si>
-    <t>TestResultExcelFilePath</t>
-  </si>
-  <si>
     <t>worksheetNo</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
   </si>
   <si>
     <t>46,365.80</t>
-  </si>
-  <si>
-    <t>F:\\Automation_TestResults\\Payroll_Tax_NI_Directors_TestReports 201819\\201819 Payroll National Insurance calculation Test result.xlsx</t>
   </si>
   <si>
     <t>66,170.00</t>
@@ -220,7 +214,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,43 +261,43 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -321,10 +314,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -359,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,7 +404,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,7 +509,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -525,13 +518,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -541,7 +534,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -550,7 +543,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -559,7 +552,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -569,12 +562,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -605,7 +598,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -624,7 +617,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -636,19 +629,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -679,7 +672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -693,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -707,7 +700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -721,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -735,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -749,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="75" r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -773,27 +766,27 @@
       <c r="E13" s="4"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="42.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,13 +814,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -838,13 +831,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>20</v>
@@ -855,13 +848,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
@@ -873,13 +866,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>20</v>
@@ -891,13 +884,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>20</v>
@@ -909,13 +902,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>20</v>
@@ -927,13 +920,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>20</v>
@@ -945,13 +938,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
@@ -963,13 +956,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>20</v>
@@ -980,37 +973,36 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C2:C10"/>
+    <ignoredError sqref="C2:C10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="50.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="50.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -1039,379 +1031,348 @@
         <v>35</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="60" r="2" s="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="6" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="50.25" r="3" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="48.75" r="4" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="33.75" r="5" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="6" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="48.75" r="6" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="44.25" r="7" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="52.5" r="8" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="55.5" r="9" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="55.5" r="10" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="G10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId10" ref="A2"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId11" ref="A3:A10"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId10" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="A3:A10" r:id="rId11" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId12" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="54.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="22.28515625" collapsed="true"/>
+    <col min="1" max="1" width="49.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.28515625" style="4" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -1440,64 +1401,58 @@
         <v>35</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="8" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="H2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="K2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TestResultExcelFilePath parameter is removed from NI Payroll class
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515"/>
+    <workbookView windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="62">
   <si>
     <t>TC</t>
   </si>
@@ -214,6 +214,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,43 +262,43 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -314,10 +315,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -352,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -509,7 +510,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -518,13 +519,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -534,7 +535,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -543,7 +544,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -552,7 +553,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -562,12 +563,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -598,7 +599,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -617,7 +618,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -629,7 +630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -638,10 +639,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -672,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -686,7 +687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -700,7 +701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -714,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -728,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -742,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -766,13 +767,13 @@
       <c r="E13" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -781,12 +782,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -973,16 +974,16 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:C10" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C2:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -991,18 +992,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="60" r="2" s="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>50</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="50.25" r="3" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>50</v>
       </c>
@@ -1107,7 +1108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="48.75" r="4" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="33.75" r="5" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>50</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="48.75" r="6" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>50</v>
       </c>
@@ -1203,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="44.25" r="7" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>50</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="52.5" r="8" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>50</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.5" r="9" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>50</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.5" r="10" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
@@ -1333,25 +1334,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId10" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="A3:A10" r:id="rId11" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId10" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId11" ref="A3:A10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId12" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -1360,19 +1361,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="49.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>50</v>
       </c>
@@ -1450,9 +1451,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>